<commit_message>
agregada argentina,tipo de facturacion y conversion de MXN a dolar
</commit_message>
<xml_diff>
--- a/server/template/plantilla_ecuador.xlsx
+++ b/server/template/plantilla_ecuador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anahil Quijada\EXCEL-COMPARE-INVOICE\excel-compare-frontend\server\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4E4966F-46F7-4D90-83AC-0877EB1CF4B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37171D2D-C663-4F3B-BD5A-8A6A5B69794D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{673C616D-76A6-457F-ACA4-A7507C6C5169}"/>
   </bookViews>
@@ -24,249 +24,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9178EE78-DFD9-456C-8E12-AC30485B9B74}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAdI
-56985    (2024-01-01 21:04:46)
-Razón Social que está en Odoo.
-En caso de que necesiten por RUT, se debe cambiar el nombre de este campo a 
-partner_id_vat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{75CB3EBD-AB13-41D2-9103-2007CB1EA4F1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAdM
-56985    (2024-01-01 21:04:46)
-Viene con fórmula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{6B6A8DDE-C8D2-41C5-B9BA-0F1545A72A2F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAck
-56985    (2024-01-01 21:04:46)
-Viene con fórmula</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{BE97A3D5-1735-4874-9810-754A18C74CB1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAdo
-56985    (2024-01-01 21:04:46)
-Siempre debe ser Facturas de cliente</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E9C1C18B-DD3A-414D-B700-2C82849FF009}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAc4
-56985    (2024-01-01 21:04:46)
-Moneda de la transacción
-Chile - CLP
-Peru - SOL</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{6E6A8312-C32B-45F8-AC07-434832FAD6AD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcc
-56985    (2024-01-01 21:04:46)
-Línea de producto</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B66C95B7-C46B-41F5-B7DE-E75A4CD4D833}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcY
-56985    (2024-01-01 21:04:46)
-Debe ser el Mes de Consumo a cobrar + Año
-Ejemplo Formato:
-Octubre 2022</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{92127822-E239-4887-B071-60ACA3C8B592}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcs
-56985    (2024-01-01 21:04:46)
-Cantidad.
-Para Conectividad Gestionada debe ser 1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{1711EFBD-39BA-4BE4-AE42-84BCDA15C0E0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcU
-56985    (2024-01-01 21:04:46)
-Precio Unitario
-Debe ser Base imponible</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{7F94065D-4937-4A94-9968-424A78DE45F2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcw
-56985    (2024-01-01 21:04:46)
-Impuestos
-Debe ser 
-IVA 19% Venta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{F1DD22AA-E181-4BFB-BD16-BBC68B8FC349}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAdw
-56985    (2024-01-01 21:04:46)
-Debe ser en porcentaje, escrbiendo el número correspondiente</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{92D34262-4F7E-4EA4-8CE2-AB695987899D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAcg
-56985    (2024-01-01 21:04:46)
-Categoría
-Debe ser Conectividad Gestionada
-Este campo ayudará a separar por categorías las facturas (Plataformas, Conectividad, etc).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{F353B35D-17A5-4ECA-8C5F-7B1C73377433}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>======
-ID#AAABDMqKAdc
-56985    (2024-01-01 21:04:46)
-Notas extras</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
@@ -319,23 +76,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,11 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,64 +420,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617D8A47-F9EA-4E44-A5AB-C6B9B2D6E2D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617D8A47-F9EA-4E44-A5AB-C6B9B2D6E2D2}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>